<commit_message>
Python Input Time Matrix Uptated
</commit_message>
<xml_diff>
--- a/states_experiences/states.xlsx
+++ b/states_experiences/states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\GitHub\bolsa_meu\states_experiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E87818E-D49B-4DB1-9557-A86E6F6AED5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458B1B00-6FBB-4470-9DAF-EB019B4CAFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projetos" sheetId="1" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
   <dimension ref="A1:AO37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1364,7 @@
   <dimension ref="A1:AO37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +1886,7 @@
   <dimension ref="A1:AO37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5915,7 +5915,7 @@
   <dimension ref="A1:AP1284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15068,7 +15068,7 @@
   <dimension ref="A1:AP1284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24220,8 +24220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9443A2C-A03B-4F5C-8CE9-B5C8C855F053}">
   <dimension ref="A2:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>